<commit_message>
refactor(common): standardize Zod schemas to camelCase
- Rename all Zod schemas to camelCase convention
- Remove redundant comments and consolidate error types
- Improve code consistency
</commit_message>
<xml_diff>
--- a/test-data/cars-invalid-update.xlsx
+++ b/test-data/cars-invalid-update.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -476,7 +476,7 @@
         <v>25000</v>
       </c>
       <c r="E4">
-        <v>1900</v>
+        <v>1800</v>
       </c>
       <c r="F4" t="str">
         <v>red</v>
@@ -704,9 +704,29 @@
         <v>black</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>NONEXIST-SKU-9999-XXX</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Ghost</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Phantom</v>
+      </c>
+      <c r="D17">
+        <v>99999</v>
+      </c>
+      <c r="E17">
+        <v>2023</v>
+      </c>
+      <c r="F17" t="str">
+        <v>black</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>